<commit_message>
ash to ash,dust to dust
</commit_message>
<xml_diff>
--- a/savingTaxProject/web/board_uploadFiles/ff.xlsx
+++ b/savingTaxProject/web/board_uploadFiles/ff.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="333">
   <si>
     <t>■ 부가가치세법 시행규칙 [별지 제21호 서식] &lt;개정 2015.3.6&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1327,10 +1327,49 @@
     <t>2017년</t>
   </si>
   <si>
+    <t>제 2 분기</t>
+  </si>
+  <si>
+    <t>7 월 01 일 ~ 12 월 31 일</t>
+  </si>
+  <si>
     <t>일반고깃집</t>
   </si>
   <si>
-    <t>서울시 강남구 역삼동 135-34</t>
+    <t>이일반</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>99/05/05</t>
+  </si>
+  <si>
+    <t>010-7777-7777</t>
+  </si>
+  <si>
+    <t>01342/서울시 강남구 역삼동/서울시 강남구 역삼동 135-34</t>
+  </si>
+  <si>
+    <t>jsmi2@jsmi.com</t>
   </si>
   <si>
     <t>2200000</t>
@@ -1373,9 +1412,6 @@
   </si>
   <si>
     <t>보건</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>123-81-12345</t>
@@ -3514,17 +3550,17 @@
         <v>4</v>
       </c>
       <c r="B8" s="100" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C8" s="100"/>
       <c r="D8" s="100" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
       <c r="G8" s="100"/>
       <c r="H8" s="83" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I8" s="83"/>
       <c r="J8" s="83"/>
@@ -3540,10 +3576,10 @@
       <c r="B9" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="141" t="s">
-        <v>303</v>
-      </c>
-      <c r="D9" s="142"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="142" t="s">
+        <v>305</v>
+      </c>
       <c r="E9" s="142"/>
       <c r="F9" s="142"/>
       <c r="G9" s="142"/>
@@ -3554,30 +3590,58 @@
         <v>8</v>
       </c>
       <c r="L9" s="141"/>
-      <c r="M9" s="142"/>
+      <c r="M9" s="142" t="s">
+        <v>306</v>
+      </c>
       <c r="N9" s="142"/>
       <c r="O9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="9"/>
+      <c r="P9" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="AA9" s="9" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row customHeight="1" ht="13.5" r="10" spans="1:27">
       <c r="A10" s="81"/>
       <c r="B10" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="125"/>
+      <c r="C10" s="125" t="s">
+        <v>314</v>
+      </c>
       <c r="D10" s="143"/>
       <c r="E10" s="144"/>
       <c r="F10" s="144"/>
@@ -3632,7 +3696,9 @@
       <c r="R11" s="99"/>
       <c r="S11" s="99"/>
       <c r="T11" s="99"/>
-      <c r="U11" s="99"/>
+      <c r="U11" s="99" t="s">
+        <v>315</v>
+      </c>
       <c r="V11" s="99"/>
       <c r="W11" s="99"/>
       <c r="X11" s="99"/>
@@ -3647,7 +3713,7 @@
       </c>
       <c r="C12" s="131"/>
       <c r="D12" s="132" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="E12" s="133"/>
       <c r="F12" s="133"/>
@@ -3664,7 +3730,9 @@
       </c>
       <c r="P12" s="135"/>
       <c r="Q12" s="136"/>
-      <c r="R12" s="137"/>
+      <c r="R12" s="137" t="s">
+        <v>317</v>
+      </c>
       <c r="S12" s="138"/>
       <c r="T12" s="138"/>
       <c r="U12" s="138"/>
@@ -3766,7 +3834,7 @@
         <v>41</v>
       </c>
       <c r="M16" s="99" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="N16" s="99"/>
       <c r="O16" s="99"/>
@@ -3776,7 +3844,7 @@
       <c r="Q16" s="99"/>
       <c r="R16" s="99"/>
       <c r="S16" s="99" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="T16" s="99"/>
       <c r="U16" s="99"/>
@@ -3840,7 +3908,7 @@
         <v>43</v>
       </c>
       <c r="M18" s="99" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="N18" s="99"/>
       <c r="O18" s="99"/>
@@ -3850,7 +3918,7 @@
       <c r="Q18" s="99"/>
       <c r="R18" s="99"/>
       <c r="S18" s="99" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="T18" s="99"/>
       <c r="U18" s="99"/>
@@ -3879,7 +3947,7 @@
         <v>44</v>
       </c>
       <c r="M19" s="99" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="N19" s="99"/>
       <c r="O19" s="99"/>
@@ -3887,7 +3955,7 @@
       <c r="Q19" s="99"/>
       <c r="R19" s="99"/>
       <c r="S19" s="99" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="T19" s="99"/>
       <c r="U19" s="99"/>
@@ -4054,7 +4122,7 @@
         <v>49</v>
       </c>
       <c r="M24" s="99" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="N24" s="99"/>
       <c r="O24" s="99"/>
@@ -4064,7 +4132,7 @@
       <c r="Q24" s="99"/>
       <c r="R24" s="99"/>
       <c r="S24" s="99" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="T24" s="99"/>
       <c r="U24" s="99"/>
@@ -4097,7 +4165,7 @@
         <v>50</v>
       </c>
       <c r="M25" s="126" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="N25" s="126"/>
       <c r="O25" s="126"/>
@@ -4105,7 +4173,7 @@
       <c r="Q25" s="99"/>
       <c r="R25" s="99"/>
       <c r="S25" s="126" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="T25" s="126"/>
       <c r="U25" s="126"/>
@@ -4233,7 +4301,7 @@
         <v>54</v>
       </c>
       <c r="M29" s="99" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="N29" s="99"/>
       <c r="O29" s="99"/>
@@ -4241,7 +4309,7 @@
       <c r="Q29" s="99"/>
       <c r="R29" s="99"/>
       <c r="S29" s="99" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="T29" s="99"/>
       <c r="U29" s="99"/>
@@ -4454,7 +4522,7 @@
         <v>87</v>
       </c>
       <c r="M35" s="99" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="N35" s="99"/>
       <c r="O35" s="99"/>
@@ -4462,7 +4530,7 @@
       <c r="Q35" s="99"/>
       <c r="R35" s="99"/>
       <c r="S35" s="99" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="T35" s="99"/>
       <c r="U35" s="99"/>
@@ -4491,7 +4559,7 @@
         <v>88</v>
       </c>
       <c r="M36" s="99" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="N36" s="99"/>
       <c r="O36" s="99"/>
@@ -4501,7 +4569,7 @@
       <c r="Q36" s="99"/>
       <c r="R36" s="99"/>
       <c r="S36" s="99" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="T36" s="99"/>
       <c r="U36" s="99"/>
@@ -4745,7 +4813,7 @@
       <c r="Q43" s="99"/>
       <c r="R43" s="99"/>
       <c r="S43" s="99" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="T43" s="99"/>
       <c r="U43" s="99"/>
@@ -4936,10 +5004,10 @@
     </row>
     <row customHeight="1" ht="18" r="52" spans="1:27" thickBot="1">
       <c r="A52" s="10" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="C52" s="80"/>
       <c r="D52" s="81"/>
@@ -5432,7 +5500,7 @@
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="48"/>
@@ -5711,12 +5779,12 @@
         <v>195</v>
       </c>
       <c r="I17" s="155" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="J17" s="204"/>
       <c r="K17" s="59"/>
       <c r="L17" s="155" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="M17" s="156"/>
     </row>
@@ -5753,14 +5821,14 @@
         <v>199</v>
       </c>
       <c r="I19" s="155" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="J19" s="204"/>
       <c r="K19" s="59" t="s">
         <v>200</v>
       </c>
       <c r="L19" s="155" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="M19" s="156"/>
     </row>

</xml_diff>